<commit_message>
ng: add kano forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Nigeria/2024/mar_2024/ng_lf_tas_202403_1_site_bay.xlsx
+++ b/LF/TAS/Nigeria/2024/mar_2024/ng_lf_tas_202403_1_site_bay.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Nigeria\2024\mar_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bonhe\Repositories\dsa-forms\LF\TAS\Nigeria\2024\mar_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE76730-00D5-4CEC-B048-21DDE07BFC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E584D990-99E9-4931-B02D-AF7B49150DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -696,7 +696,7 @@
     <font>
       <sz val="8"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1132,11 +1132,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:XFD3"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1540,8 +1540,8 @@
   <dimension ref="A1:G133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD13"/>
+      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A94" sqref="A94:XFD97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3374,7 +3374,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>